<commit_message>
Added check/logic for players in year 2 or 3 on new contract to only have vet min 1 year deal
</commit_message>
<xml_diff>
--- a/Files/Madden25/IE/Season9/ExpectedContractLength.xlsx
+++ b/Files/Madden25/IE/Season9/ExpectedContractLength.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/MaddenTools/Files/Madden24/IE/Season3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40f61192ff96ff75/Documents/Git/MaddenTools/Files/Madden25/IE/Season9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5946" documentId="13_ncr:1_{ADED6FFD-BF9D-425E-B0E9-69FF67D7C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D0A1E7A-A35E-4CC5-A084-91FE4933959B}"/>
+  <xr:revisionPtr revIDLastSave="6021" documentId="13_ncr:1_{ADED6FFD-BF9D-425E-B0E9-69FF67D7C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DA195FB-21C0-453B-97D0-CDB7E1B5304B}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="24" r:id="rId1"/>
@@ -163,10 +163,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,16 +489,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6200DA08-E509-45AF-AE2B-CB0FB74399A3}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -516,12 +512,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>99</v>
@@ -530,21 +526,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -558,7 +554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -572,7 +568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -586,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -600,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -614,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -628,7 +624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -642,12 +638,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C11">
         <v>99</v>
@@ -656,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -664,13 +660,13 @@
         <v>74</v>
       </c>
       <c r="C12">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -684,12 +680,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C14">
         <v>99</v>
@@ -698,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -706,18 +702,18 @@
         <v>87</v>
       </c>
       <c r="C15">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="1">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16">
         <v>86</v>
@@ -726,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -734,13 +730,13 @@
         <v>74</v>
       </c>
       <c r="C17">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -754,12 +750,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="1">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C19">
         <v>99</v>
@@ -768,35 +764,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="1">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C20">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="1">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -804,13 +800,13 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -824,12 +820,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24">
         <v>89</v>
@@ -838,7 +834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -846,13 +842,13 @@
         <v>74</v>
       </c>
       <c r="C25">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -866,7 +862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -880,12 +876,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C28">
         <v>99</v>
@@ -894,35 +890,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="1">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C29">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="1">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -930,13 +926,13 @@
         <v>70</v>
       </c>
       <c r="C31">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -950,12 +946,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="1">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C33">
         <v>99</v>
@@ -964,49 +960,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="1">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C34">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
       <c r="B35" s="1">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
       <c r="B36" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1014,18 +1010,18 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C38">
         <v>99</v>
@@ -1034,35 +1030,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="1">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C39">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="1">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1070,13 +1066,13 @@
         <v>70</v>
       </c>
       <c r="C41">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -1104,12 +1100,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44">
         <v>89</v>
@@ -1118,7 +1114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1126,18 +1122,18 @@
         <v>74</v>
       </c>
       <c r="C45">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>8</v>
       </c>
       <c r="B46" s="1">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C46">
         <v>73</v>
@@ -1146,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -1154,18 +1150,18 @@
         <v>1</v>
       </c>
       <c r="C47">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
       <c r="B48" s="1">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C48">
         <v>99</v>
@@ -1174,7 +1170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1182,18 +1178,18 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D49">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50">
         <v>82</v>
@@ -1202,7 +1198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1210,13 +1206,13 @@
         <v>70</v>
       </c>
       <c r="C51">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1230,12 +1226,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
       <c r="B53" s="1">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C53">
         <v>99</v>
@@ -1244,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1252,18 +1248,18 @@
         <v>83</v>
       </c>
       <c r="C54">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D54">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
       <c r="B55" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55">
         <v>82</v>
@@ -1272,7 +1268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -1280,13 +1276,13 @@
         <v>70</v>
       </c>
       <c r="C56">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -1300,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -1314,7 +1310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -1328,12 +1324,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60">
         <v>83</v>
@@ -1342,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -1350,13 +1346,13 @@
         <v>70</v>
       </c>
       <c r="C61">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -1370,12 +1366,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
       <c r="B63" s="1">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C63">
         <v>99</v>
@@ -1384,7 +1380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -1392,13 +1388,13 @@
         <v>80</v>
       </c>
       <c r="C64">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D64">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -1426,12 +1422,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>13</v>
       </c>
       <c r="B67" s="1">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C67">
         <v>99</v>
@@ -1440,7 +1436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -1448,13 +1444,13 @@
         <v>88</v>
       </c>
       <c r="C68">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D68">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -1468,12 +1464,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>13</v>
       </c>
       <c r="B70" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C70">
         <v>79</v>
@@ -1482,7 +1478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -1490,18 +1486,18 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>14</v>
       </c>
       <c r="B72" s="1">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C72">
         <v>99</v>
@@ -1510,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -1518,13 +1514,13 @@
         <v>80</v>
       </c>
       <c r="C73">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D73">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>14</v>
       </c>
@@ -1538,7 +1534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -1552,12 +1548,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>15</v>
       </c>
       <c r="B76" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C76">
         <v>99</v>
@@ -1566,7 +1562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>15</v>
       </c>
@@ -1574,13 +1570,13 @@
         <v>85</v>
       </c>
       <c r="C77">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D77">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>15</v>
       </c>
@@ -1594,7 +1590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>15</v>
       </c>
@@ -1608,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>15</v>
       </c>
@@ -1622,7 +1618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -1636,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -1650,12 +1646,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>16</v>
       </c>
       <c r="B83" s="1">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C83">
         <v>79</v>
@@ -1664,7 +1660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -1672,13 +1668,13 @@
         <v>1</v>
       </c>
       <c r="C84">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D84">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -1692,7 +1688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -1706,12 +1702,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>17</v>
       </c>
       <c r="B87" s="1">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C87">
         <v>79</v>
@@ -1720,7 +1716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -1728,13 +1724,13 @@
         <v>1</v>
       </c>
       <c r="C88">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D88">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -1748,7 +1744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -1762,12 +1758,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>18</v>
       </c>
       <c r="B91" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C91">
         <v>77</v>
@@ -1776,7 +1772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -1784,13 +1780,13 @@
         <v>72</v>
       </c>
       <c r="C92">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D92">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>18</v>
       </c>
@@ -1804,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -1818,7 +1814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>19</v>
       </c>
@@ -1832,7 +1828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -1846,7 +1842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>19</v>
       </c>

</xml_diff>